<commit_message>
bot working on server
</commit_message>
<xml_diff>
--- a/meetings_dumped/dombrovskis.xlsx
+++ b/meetings_dumped/dombrovskis.xlsx
@@ -3121,12 +3121,13 @@
       </c>
       <c r="C44" s="529" t="inlineStr">
         <is>
-          <t>The Blackstone Group</t>
+          <t>Bloomberg L.P.</t>
         </is>
       </c>
       <c r="D44" s="529" t="inlineStr">
         <is>
-          <t xml:space="preserve">Capital Markets Union; Sustainable finance </t>
+          <t xml:space="preserve">EU-US relations; Sustainable finance; Trade and Technology Council; Artificial Intelligence, Cybersecurity and Data skills 
+ </t>
         </is>
       </c>
     </row>
@@ -3143,13 +3144,12 @@
       </c>
       <c r="C45" s="529" t="inlineStr">
         <is>
-          <t>Bloomberg L.P.</t>
+          <t>The Blackstone Group</t>
         </is>
       </c>
       <c r="D45" s="529" t="inlineStr">
         <is>
-          <t xml:space="preserve">EU-US relations; Sustainable finance; Trade and Technology Council; Artificial Intelligence, Cybersecurity and Data skills 
- </t>
+          <t xml:space="preserve">Capital Markets Union; Sustainable finance </t>
         </is>
       </c>
     </row>
@@ -3231,15 +3231,38 @@
       </c>
       <c r="B49" s="529" t="inlineStr">
         <is>
+          <t xml:space="preserve">video conference </t>
+        </is>
+      </c>
+      <c r="C49" s="529" t="inlineStr">
+        <is>
+          <t>Microsoft Corporation</t>
+        </is>
+      </c>
+      <c r="D49" s="529" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The main topics for the meeting were: transatlantic relations with a focus on US-EU Trade and Technology Council; digital trade and WTO e-commerce negotiations; Digital angle of economic recovery. 
+  </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="526" t="inlineStr">
+        <is>
+          <t>29/06/2021</t>
+        </is>
+      </c>
+      <c r="B50" s="529" t="inlineStr">
+        <is>
           <t>virtual</t>
         </is>
       </c>
-      <c r="C49" s="529" t="inlineStr">
+      <c r="C50" s="529" t="inlineStr">
         <is>
           <t>CEMBUREAU - The European Cement Association, TITAN CEMENT INTERNATIONAL SA, CRH plc</t>
         </is>
       </c>
-      <c r="D49" s="529" t="inlineStr">
+      <c r="D50" s="529" t="inlineStr">
         <is>
           <t xml:space="preserve">- EU cement industry's decarbonisation efforts
 - Fit for 55, trade and carbon leakage
@@ -3247,29 +3270,6 @@
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="526" t="inlineStr">
-        <is>
-          <t>29/06/2021</t>
-        </is>
-      </c>
-      <c r="B50" s="529" t="inlineStr">
-        <is>
-          <t xml:space="preserve">video conference </t>
-        </is>
-      </c>
-      <c r="C50" s="529" t="inlineStr">
-        <is>
-          <t>Microsoft Corporation</t>
-        </is>
-      </c>
-      <c r="D50" s="529" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The main topics for the meeting were: transatlantic relations with a focus on US-EU Trade and Technology Council; digital trade and WTO e-commerce negotiations; Digital angle of economic recovery. 
-  </t>
-        </is>
-      </c>
-    </row>
     <row r="51">
       <c r="A51" s="526" t="inlineStr">
         <is>
@@ -3300,17 +3300,18 @@
       </c>
       <c r="B52" s="529" t="inlineStr">
         <is>
-          <t xml:space="preserve">video conference </t>
+          <t>video-conference</t>
         </is>
       </c>
       <c r="C52" s="529" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Association des Constructeurs Européens d'Automobiles</t>
         </is>
       </c>
       <c r="D52" s="529" t="inlineStr">
         <is>
-          <t xml:space="preserve">Trade policy, including transatlantic trade relations - EU-US Trade and Technology initiative, digital payments and cross border data flows. </t>
+          <t xml:space="preserve">Trade policy review; Steel safeguard review; EU-US relations; Fit for 55 preparation
+</t>
         </is>
       </c>
     </row>
@@ -3322,18 +3323,17 @@
       </c>
       <c r="B53" s="529" t="inlineStr">
         <is>
-          <t>video-conference</t>
+          <t xml:space="preserve">video conference </t>
         </is>
       </c>
       <c r="C53" s="529" t="inlineStr">
         <is>
-          <t>Association des Constructeurs Européens d'Automobiles</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="D53" s="529" t="inlineStr">
         <is>
-          <t xml:space="preserve">Trade policy review; Steel safeguard review; EU-US relations; Fit for 55 preparation
-</t>
+          <t xml:space="preserve">Trade policy, including transatlantic trade relations - EU-US Trade and Technology initiative, digital payments and cross border data flows. </t>
         </is>
       </c>
     </row>

</xml_diff>